<commit_message>
Updated Molprobity statistics to match latest commits
</commit_message>
<xml_diff>
--- a/MolprobityStatistics.xlsx
+++ b/MolprobityStatistics.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="25516"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="16060" tabRatio="500"/>
+    <workbookView xWindow="1320" yWindow="0" windowWidth="25600" windowHeight="16060" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -1245,36 +1245,6 @@
       <alignment horizontal="left" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="10" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="1" fillId="11" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="11" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="11" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="11" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="11" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="11" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="11" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="11" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="11" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="11" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="11" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1293,11 +1263,41 @@
     <xf numFmtId="0" fontId="5" fillId="4" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="11" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="11" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="11" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="11" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="11" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="11" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="11" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="11" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="11" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="11" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="11" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="11" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="13">
@@ -1645,7 +1645,7 @@
   <dimension ref="A1:M74"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B1" sqref="B1"/>
+      <selection activeCell="M8" sqref="M8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -1664,76 +1664,76 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:13" ht="24" thickBot="1">
-      <c r="D1" s="92" t="s">
+      <c r="D1" s="82" t="s">
         <v>8</v>
       </c>
-      <c r="E1" s="93"/>
-      <c r="F1" s="93"/>
-      <c r="G1" s="93"/>
-      <c r="H1" s="94"/>
-      <c r="I1" s="92" t="s">
+      <c r="E1" s="83"/>
+      <c r="F1" s="83"/>
+      <c r="G1" s="83"/>
+      <c r="H1" s="84"/>
+      <c r="I1" s="82" t="s">
         <v>9</v>
       </c>
-      <c r="J1" s="93"/>
-      <c r="K1" s="93"/>
-      <c r="L1" s="93"/>
-      <c r="M1" s="95"/>
+      <c r="J1" s="83"/>
+      <c r="K1" s="83"/>
+      <c r="L1" s="83"/>
+      <c r="M1" s="85"/>
     </row>
     <row r="2" spans="1:13" s="79" customFormat="1">
-      <c r="A2" s="80" t="s">
+      <c r="A2" s="92" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="82" t="s">
+      <c r="B2" s="94" t="s">
         <v>1</v>
       </c>
-      <c r="C2" s="84" t="s">
+      <c r="C2" s="96" t="s">
         <v>2</v>
       </c>
-      <c r="D2" s="86" t="s">
+      <c r="D2" s="90" t="s">
         <v>3</v>
       </c>
-      <c r="E2" s="88" t="s">
+      <c r="E2" s="86" t="s">
         <v>4</v>
       </c>
-      <c r="F2" s="88" t="s">
+      <c r="F2" s="86" t="s">
         <v>5</v>
       </c>
-      <c r="G2" s="88" t="s">
+      <c r="G2" s="86" t="s">
         <v>6</v>
       </c>
-      <c r="H2" s="96" t="s">
+      <c r="H2" s="88" t="s">
         <v>7</v>
       </c>
-      <c r="I2" s="86" t="s">
+      <c r="I2" s="90" t="s">
         <v>3</v>
       </c>
-      <c r="J2" s="88" t="s">
+      <c r="J2" s="86" t="s">
         <v>4</v>
       </c>
-      <c r="K2" s="88" t="s">
+      <c r="K2" s="86" t="s">
         <v>5</v>
       </c>
-      <c r="L2" s="88" t="s">
+      <c r="L2" s="86" t="s">
         <v>6</v>
       </c>
-      <c r="M2" s="90" t="s">
+      <c r="M2" s="80" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="3" spans="1:13" s="79" customFormat="1" ht="16" thickBot="1">
-      <c r="A3" s="81"/>
-      <c r="B3" s="83"/>
-      <c r="C3" s="85"/>
-      <c r="D3" s="87"/>
-      <c r="E3" s="89"/>
-      <c r="F3" s="89"/>
-      <c r="G3" s="89"/>
-      <c r="H3" s="97"/>
-      <c r="I3" s="87"/>
-      <c r="J3" s="89"/>
-      <c r="K3" s="89"/>
-      <c r="L3" s="89"/>
-      <c r="M3" s="91"/>
+      <c r="A3" s="93"/>
+      <c r="B3" s="95"/>
+      <c r="C3" s="97"/>
+      <c r="D3" s="91"/>
+      <c r="E3" s="87"/>
+      <c r="F3" s="87"/>
+      <c r="G3" s="87"/>
+      <c r="H3" s="89"/>
+      <c r="I3" s="91"/>
+      <c r="J3" s="87"/>
+      <c r="K3" s="87"/>
+      <c r="L3" s="87"/>
+      <c r="M3" s="81"/>
     </row>
     <row r="4" spans="1:13">
       <c r="A4" s="7" t="s">
@@ -1880,19 +1880,19 @@
         <v>34</v>
       </c>
       <c r="I7" s="50">
-        <v>0.56000000000000005</v>
+        <v>0.48</v>
       </c>
       <c r="J7" s="62">
         <v>99</v>
       </c>
       <c r="K7" s="63">
-        <v>1.0200000000000001E-2</v>
+        <v>5.11E-2</v>
       </c>
       <c r="L7" s="62">
-        <v>1.21</v>
+        <v>1.51</v>
       </c>
       <c r="M7" s="64">
-        <v>99</v>
+        <v>95</v>
       </c>
     </row>
     <row r="8" spans="1:13">
@@ -4575,7 +4575,7 @@
       </c>
       <c r="I74" s="54">
         <f t="shared" si="0"/>
-        <v>0.94542857142857128</v>
+        <v>0.94428571428571417</v>
       </c>
       <c r="J74" s="54">
         <f t="shared" si="0"/>
@@ -4583,19 +4583,24 @@
       </c>
       <c r="K74" s="58">
         <f t="shared" si="0"/>
-        <v>3.7967142857142845E-2</v>
+        <v>3.8551428571428563E-2</v>
       </c>
       <c r="L74" s="54">
         <f t="shared" si="0"/>
-        <v>1.5565714285714281</v>
+        <v>1.5608571428571425</v>
       </c>
       <c r="M74" s="56">
         <f t="shared" si="0"/>
-        <v>90.01428571428572</v>
+        <v>89.957142857142856</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="15">
+    <mergeCell ref="A2:A3"/>
+    <mergeCell ref="B2:B3"/>
+    <mergeCell ref="C2:C3"/>
+    <mergeCell ref="D2:D3"/>
+    <mergeCell ref="E2:E3"/>
     <mergeCell ref="M2:M3"/>
     <mergeCell ref="D1:H1"/>
     <mergeCell ref="I1:M1"/>
@@ -4606,11 +4611,6 @@
     <mergeCell ref="K2:K3"/>
     <mergeCell ref="L2:L3"/>
     <mergeCell ref="F2:F3"/>
-    <mergeCell ref="A2:A3"/>
-    <mergeCell ref="B2:B3"/>
-    <mergeCell ref="C2:C3"/>
-    <mergeCell ref="D2:D3"/>
-    <mergeCell ref="E2:E3"/>
   </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>

</xml_diff>